<commit_message>
- ext-abstractive slurm script added
</commit_message>
<xml_diff>
--- a/results/results_summary.xlsx
+++ b/results/results_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keert\PycharmProjects\PreSumm\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{475D0C5D-BC3E-4FD1-9A33-06668398AC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54549D8F-C7C0-4E8B-9D7F-11FAFB3445EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3300" windowWidth="29040" windowHeight="15720" xr2:uid="{63201BA6-9AF6-4939-ACFF-6857212007B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{63201BA6-9AF6-4939-ACFF-6857212007B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>Training data</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>ROUGE - SU*</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>cnndm_baseline_best.pt</t>
+  </si>
+  <si>
+    <t>Abstractive</t>
+  </si>
+  <si>
+    <t>BertExtAbs</t>
+  </si>
+  <si>
+    <t>BertAbs</t>
+  </si>
+  <si>
+    <t>bertextabs_cnndm_final_148000.pt</t>
+  </si>
+  <si>
+    <t>xsum</t>
+  </si>
+  <si>
+    <t>bertextabs_xsum_final_30000.pt</t>
   </si>
 </sst>
 </file>
@@ -137,13 +161,131 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="38">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -154,6 +296,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1860824E-F391-4060-8B10-27408DFB6EA2}" name="Table1" displayName="Table1" ref="A1:R27" headerRowDxfId="18" dataDxfId="19">
+  <autoFilter ref="A1:R27" xr:uid="{1860824E-F391-4060-8B10-27408DFB6EA2}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{87AF1AD0-1B2B-4173-A91B-EEACF9B5D99E}" name="Index" totalsRowLabel="Total" dataDxfId="37" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{98D75078-1F4F-4F02-A58A-28546DC0C21B}" name="Summarization" dataDxfId="36" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E7501773-6FA9-44F5-B28D-B5C559825576}" name="Setting" dataDxfId="35" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7661FD5D-9F07-458A-A141-69C4B97F6ABB}" name="Training data" dataDxfId="34" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{37880DBB-D331-4CA6-8B85-D2021401D7DB}" name="Initializer" dataDxfId="33" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{30609B29-51E6-4F67-BE3B-4E7DAE49A666}" name="Initializer iterations" dataDxfId="32" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{AD7375E7-1F0F-4D51-86A2-F7F0C74BEF6B}" name="Test data" dataDxfId="31" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{49DB5E94-C84F-47B5-B90E-3FEB711BFB53}" name="New iterations" dataDxfId="30" totalsRowDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{A872158E-5F7C-4C97-A5C6-16641DA953AE}" name="ROUGE - 1" dataDxfId="29" totalsRowDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{F470CBEA-18B3-4077-B3D5-DD0820A2CD41}" name="ROUGE - 2" dataDxfId="28" totalsRowDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{55BDA761-C780-4853-977E-001E1011414E}" name="ROUGE - 3" dataDxfId="27" totalsRowDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{7F8B37E8-3008-4A71-BC58-7BB6738A5C3F}" name="ROUGE - 4" dataDxfId="26" totalsRowDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{81D742B6-53EA-42CA-97A9-F503D9055D8B}" name="ROUGE - L" dataDxfId="25" totalsRowDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{1C8D4612-CC68-43E2-914B-2CC840D838F5}" name="ROUGE - W-1.2" dataDxfId="24" totalsRowDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{83CA91FC-7C27-4CEB-AE38-BB0298E8BFFE}" name="ROUGE - S*" dataDxfId="23" totalsRowDxfId="14"/>
+    <tableColumn id="16" xr3:uid="{838E536E-CB55-439E-BC5C-D1C21E450157}" name="ROUGE - SU*" dataDxfId="22" totalsRowDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{967849D7-F537-4404-A863-1AEF8AF61D17}" name="Model save path" dataDxfId="21" totalsRowDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{DA128101-0E91-4886-BA4F-794D82F8145D}" name="Result file name" totalsRowFunction="count" dataDxfId="20" totalsRowDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,143 +622,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0AA60-5F66-4D55-8642-42D8446770FF}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="11.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1">
         <v>0.32181999999999999</v>
       </c>
-      <c r="I2">
+      <c r="J2" s="1">
         <v>0.16797000000000001</v>
       </c>
-      <c r="J2">
+      <c r="K2" s="1">
         <v>0.10191</v>
       </c>
-      <c r="K2">
+      <c r="L2" s="1">
         <v>7.1150000000000005E-2</v>
       </c>
-      <c r="L2">
+      <c r="M2" s="1">
         <v>0.28305000000000002</v>
       </c>
-      <c r="M2">
+      <c r="N2" s="1">
         <v>0.20655000000000001</v>
       </c>
-      <c r="N2">
+      <c r="O2" s="1">
         <v>0.11378000000000001</v>
       </c>
-      <c r="O2">
+      <c r="P2" s="1">
         <v>0.13144</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* further data cleaning * pytorch tutorial * results update
</commit_message>
<xml_diff>
--- a/results/results_summary.xlsx
+++ b/results/results_summary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keert\PycharmProjects\PreSumm\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8890657F-A18E-417D-8ECB-67DBF5938527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90A01CF-9C1A-4AB1-B18A-D174961DF83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{63201BA6-9AF6-4939-ACFF-6857212007B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Results" sheetId="3" r:id="rId3"/>
+    <sheet name="Results" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="87">
   <si>
     <t>Training data</t>
   </si>
@@ -166,12 +166,6 @@
     <t>abs_bertextabs_cnn_cnndm_baseline.txt</t>
   </si>
   <si>
-    <t>bertabs_cnndm_final_148000.pt</t>
-  </si>
-  <si>
-    <t>bertabs_cnndm_final_200000.pt</t>
-  </si>
-  <si>
     <t>bertext_cnndm_final_50000.pt</t>
   </si>
   <si>
@@ -212,6 +206,99 @@
   </si>
   <si>
     <t>bertext_cnndm_historical_50000.pt</t>
+  </si>
+  <si>
+    <t>results\abstractive\test_abs_cnn_148000_historical_200000.txt</t>
+  </si>
+  <si>
+    <t>/data/historical_samples_new/abstractive/basic_model_path/model_step_200000.pt</t>
+  </si>
+  <si>
+    <t>New Setting</t>
+  </si>
+  <si>
+    <t>/results/abstractive/test_abs_cnn_baseline_historical.txt</t>
+  </si>
+  <si>
+    <t>\data\historical_samples_new\model_path\abstractive\pre_model_path\model_step_250000.pt</t>
+  </si>
+  <si>
+    <t>results\abstractive\test_abs_cnn_148000_historical_250000.txt</t>
+  </si>
+  <si>
+    <t>test_cnn_baseline_20000_new.txt</t>
+  </si>
+  <si>
+    <t>data\historical_samples_new\model_path\extractive\pre_model_path\model_step_70000.pt</t>
+  </si>
+  <si>
+    <t>data\historical_samples_new\model_path\extractive\basic_model_path\model_step_50000.pt</t>
+  </si>
+  <si>
+    <t>model of index (18 )</t>
+  </si>
+  <si>
+    <t>data\historical_samples_new\model_path\extractive\retrain_model_path\model_step_70000.pt</t>
+  </si>
+  <si>
+    <t>results\extractive\test_ext_historical_50000_historical_70000.txt</t>
+  </si>
+  <si>
+    <t>results\extractive\test_ext_cnn_50000_historical_70000.txt</t>
+  </si>
+  <si>
+    <t>results\extractive\test_ext_cnn_20000_historical_50000.txt</t>
+  </si>
+  <si>
+    <t>Extractive - oracle</t>
+  </si>
+  <si>
+    <t>Extractive - Oracle</t>
+  </si>
+  <si>
+    <t>Extractive - LEAD 3</t>
+  </si>
+  <si>
+    <t>Extractive - MatchSum</t>
+  </si>
+  <si>
+    <t>CNNDM BERT</t>
+  </si>
+  <si>
+    <t>CNNDM Roberta</t>
+  </si>
+  <si>
+    <t>Multinews</t>
+  </si>
+  <si>
+    <t>Pubmed</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>Wikihow</t>
+  </si>
+  <si>
+    <t>Xsum</t>
+  </si>
+  <si>
+    <t>facebook/bart-large-cnn</t>
+  </si>
+  <si>
+    <t>Text rank - 10%</t>
+  </si>
+  <si>
+    <t>minhtoan/t5-finetune-cnndaily-news</t>
+  </si>
+  <si>
+    <t>ssheifer/distbart-cnn-12-6</t>
+  </si>
+  <si>
+    <t>google/pegasus_cnn_dailymail</t>
+  </si>
+  <si>
+    <t>sbert/paraphrase-MiniLM-L6-v2</t>
   </si>
 </sst>
 </file>
@@ -255,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,18 +357,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor theme="4" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
@@ -302,6 +377,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -317,7 +398,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -331,40 +412,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,6 +571,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2524879</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>105135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F4E20E-6250-C2E2-C2AC-8EB8151722EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1895475" y="7810500"/>
+          <a:ext cx="5401429" cy="2581635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1036,7 +1151,7 @@
         <v>14</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1092,7 +1207,7 @@
         <v>5.2109999999999997E-2</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1165,7 +1280,7 @@
         <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1">
         <v>50000</v>
@@ -1254,10 +1369,10 @@
         <v>0.12225999999999999</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1313,10 +1428,10 @@
         <v>5.2109999999999997E-2</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1327,7 +1442,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>37</v>
@@ -1631,7 +1746,7 @@
         <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G14" s="1">
         <v>200000</v>
@@ -1687,10 +1802,10 @@
         <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="G15" s="2">
         <v>30000</v>
@@ -1726,10 +1841,10 @@
         <v>7.4759999999999993E-2</v>
       </c>
       <c r="R15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S15" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -1784,248 +1899,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFCFEBE-6426-4A72-8B3E-F272ED2EB901}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBC4A20-EA1E-4D4D-BD7D-18C128FF6D9C}">
+  <dimension ref="A3:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7">
-        <v>14</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="7" t="str">
-        <f>Sheet1!R12</f>
-        <v>/data/historical_samples/abstractive/basic_model_path/model_step_200000.pt</v>
-      </c>
-      <c r="G1" s="7">
-        <v>200000</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="7">
-        <v>250000</v>
-      </c>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>15</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="8">
-        <v>148000</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="8">
-        <v>200000</v>
-      </c>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>16</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="7">
-        <v>148000</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="7">
-        <v>200000</v>
-      </c>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>17</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="9">
-        <v>200000</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="9">
-        <v>250000</v>
-      </c>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>18</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="10">
-        <v>200000</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="10">
-        <v>250000</v>
-      </c>
-      <c r="J5" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBC4A20-EA1E-4D4D-BD7D-18C128FF6D9C}">
-  <dimension ref="A3:Q23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="53" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="75" customWidth="1"/>
-    <col min="14" max="14" width="50.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="90" style="1" customWidth="1"/>
+    <col min="14" max="14" width="50.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="14"/>
-    </row>
-    <row r="5" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -2071,7 +2021,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2112,12 +2062,12 @@
         <v>14</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -2155,14 +2105,14 @@
         <v>17.847999999999999</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2199,11 +2149,11 @@
         <v>20.082999999999998</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2219,7 +2169,7 @@
         <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1">
         <v>50000</v>
@@ -2240,10 +2190,10 @@
         <v>20.654</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -2281,66 +2231,66 @@
         <v>26.693999999999999</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F12" s="3"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="14"/>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="B14" s="11"/>
+    </row>
+    <row r="16" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="M16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -2348,7 +2298,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>37</v>
@@ -2374,7 +2324,7 @@
       <c r="K17" s="2">
         <v>18.257000000000001</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="2">
         <v>30.26</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -2387,7 +2337,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>9</v>
       </c>
@@ -2421,7 +2371,7 @@
       <c r="K18" s="2">
         <v>20.507000000000001</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="2">
         <v>32.765999999999998</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -2468,7 +2418,7 @@
       <c r="K19" s="6">
         <v>8.9580000000000002</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="6">
         <v>19.163</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -2478,8 +2428,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2522,7 +2472,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -2566,8 +2516,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2583,7 +2533,7 @@
         <v>27</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G22" s="1">
         <v>200000</v>
@@ -2610,7 +2560,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2621,19 +2571,1229 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="13"/>
+      <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
+    <row r="24" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+    </row>
+    <row r="26" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="2">
+        <v>148000</v>
+      </c>
+      <c r="J30" s="2">
+        <v>28.27</v>
+      </c>
+      <c r="K30" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="L30" s="2">
+        <v>21.82</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>15</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="1">
+        <v>148000</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="1">
+        <v>200000</v>
+      </c>
+      <c r="J31" s="9">
+        <v>47.29</v>
+      </c>
+      <c r="K31" s="9">
+        <v>25.36</v>
+      </c>
+      <c r="L31" s="9">
+        <v>38.53</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="1">
+        <v>200000</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="1">
+        <v>250000</v>
+      </c>
+      <c r="J32" s="5">
+        <v>47.62</v>
+      </c>
+      <c r="K32" s="5">
+        <v>25.54</v>
+      </c>
+      <c r="L32" s="5">
+        <v>38.47</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="2">
+        <v>30.88</v>
+      </c>
+      <c r="K35" s="2">
+        <v>11.04</v>
+      </c>
+      <c r="L35" s="2">
+        <v>23.21</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" s="1">
+        <v>50000</v>
+      </c>
+      <c r="J36" s="9">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="K36" s="9">
+        <v>12.64</v>
+      </c>
+      <c r="L36" s="9">
+        <v>24.17</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="1">
+        <v>70000</v>
+      </c>
+      <c r="J37" s="9">
+        <v>32.15</v>
+      </c>
+      <c r="K37" s="9">
+        <v>12.66</v>
+      </c>
+      <c r="L37" s="9">
+        <v>24.23</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="1">
+        <v>70000</v>
+      </c>
+      <c r="J38" s="5">
+        <v>32.56</v>
+      </c>
+      <c r="K38" s="5">
+        <v>12.97</v>
+      </c>
+      <c r="L38" s="5">
+        <v>24.52</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0E80C8-B7D3-4B70-8AC9-3123A27EDC70}">
+  <dimension ref="A3:P28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="59.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2">
+        <v>148000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>28.27</v>
+      </c>
+      <c r="K4" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="L4" s="2">
+        <v>21.82</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1">
+        <v>148000</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1">
+        <v>200000</v>
+      </c>
+      <c r="J5" s="9">
+        <v>47.29</v>
+      </c>
+      <c r="K5" s="9">
+        <v>25.36</v>
+      </c>
+      <c r="L5" s="9">
+        <v>38.53</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200000</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1">
+        <v>250000</v>
+      </c>
+      <c r="J6" s="5">
+        <v>47.62</v>
+      </c>
+      <c r="K6" s="5">
+        <v>25.54</v>
+      </c>
+      <c r="L6" s="5">
+        <v>38.47</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <v>19.2</v>
+      </c>
+      <c r="K7">
+        <v>6.93</v>
+      </c>
+      <c r="L7">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8">
+        <v>24.18</v>
+      </c>
+      <c r="K8">
+        <v>5.85</v>
+      </c>
+      <c r="L8">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="K9">
+        <v>6.93</v>
+      </c>
+      <c r="L9">
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10">
+        <v>22.23</v>
+      </c>
+      <c r="K10">
+        <v>7.74</v>
+      </c>
+      <c r="L10">
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2">
+        <v>30.88</v>
+      </c>
+      <c r="K13" s="2">
+        <v>11.04</v>
+      </c>
+      <c r="L13" s="2">
+        <v>23.21</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1">
+        <v>50000</v>
+      </c>
+      <c r="J14" s="9">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="K14" s="9">
+        <v>12.64</v>
+      </c>
+      <c r="L14" s="9">
+        <v>24.17</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1">
+        <v>70000</v>
+      </c>
+      <c r="J15" s="9">
+        <v>32.15</v>
+      </c>
+      <c r="K15" s="9">
+        <v>12.66</v>
+      </c>
+      <c r="L15" s="9">
+        <v>24.23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1">
+        <v>70000</v>
+      </c>
+      <c r="J16" s="5">
+        <v>32.56</v>
+      </c>
+      <c r="K16" s="5">
+        <v>12.97</v>
+      </c>
+      <c r="L16" s="5">
+        <v>24.52</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17">
+        <v>33.6</v>
+      </c>
+      <c r="K17">
+        <v>15.81</v>
+      </c>
+      <c r="L17">
+        <v>24.94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18">
+        <v>30.13</v>
+      </c>
+      <c r="K18">
+        <v>11.84</v>
+      </c>
+      <c r="L18">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19">
+        <v>26.9</v>
+      </c>
+      <c r="K19">
+        <v>8.84</v>
+      </c>
+      <c r="L19">
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20">
+        <v>25.3</v>
+      </c>
+      <c r="K20">
+        <v>8.27</v>
+      </c>
+      <c r="L20">
+        <v>19.309999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21">
+        <v>24.68</v>
+      </c>
+      <c r="K21">
+        <v>7.64</v>
+      </c>
+      <c r="L21">
+        <v>18.93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22">
+        <v>25.56</v>
+      </c>
+      <c r="K22">
+        <v>8.35</v>
+      </c>
+      <c r="L22">
+        <v>19.54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23">
+        <v>27.9</v>
+      </c>
+      <c r="K23">
+        <v>9.06</v>
+      </c>
+      <c r="L23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24">
+        <v>26.82</v>
+      </c>
+      <c r="K24">
+        <v>8.89</v>
+      </c>
+      <c r="L24">
+        <v>20.43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25">
+        <v>27.39</v>
+      </c>
+      <c r="K25">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="L25">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26">
+        <v>25.23</v>
+      </c>
+      <c r="K26">
+        <v>8.98</v>
+      </c>
+      <c r="L26">
+        <v>18.04</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K27">
+        <v>6.91</v>
+      </c>
+      <c r="L27">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Embedding layer - ablation study
</commit_message>
<xml_diff>
--- a/results/results_summary.xlsx
+++ b/results/results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keert\PycharmProjects\PreSumm\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90A01CF-9C1A-4AB1-B18A-D174961DF83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE1B45-9A8A-42EA-B6E8-B319F59EBA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{63201BA6-9AF6-4939-ACFF-6857212007B8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="89">
   <si>
     <t>Training data</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>sbert/paraphrase-MiniLM-L6-v2</t>
+  </si>
+  <si>
+    <t>without position embeddings</t>
+  </si>
+  <si>
+    <t>without token type embeddings</t>
   </si>
 </sst>
 </file>
@@ -3050,10 +3056,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0E80C8-B7D3-4B70-8AC9-3123A27EDC70}">
-  <dimension ref="A3:P28"/>
+  <dimension ref="A3:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,45 +3253,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7">
-        <v>19.2</v>
-      </c>
-      <c r="K7">
-        <v>6.93</v>
-      </c>
-      <c r="L7">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8">
-        <v>24.18</v>
-      </c>
-      <c r="K8">
-        <v>5.85</v>
-      </c>
-      <c r="L8">
-        <v>17.61</v>
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="5">
+        <v>47.2</v>
+      </c>
+      <c r="K7" s="5">
+        <v>24.77</v>
+      </c>
+      <c r="L7" s="5">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="5">
+        <v>36</v>
+      </c>
+      <c r="K8" s="5">
+        <v>12.85</v>
+      </c>
+      <c r="L8" s="5">
+        <v>27.51</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -3293,223 +3286,176 @@
         <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="H9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J9">
-        <v>19.260000000000002</v>
+        <v>19.2</v>
       </c>
       <c r="K9">
         <v>6.93</v>
       </c>
       <c r="L9">
-        <v>13.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10">
+        <v>24.18</v>
+      </c>
+      <c r="K10">
+        <v>5.85</v>
+      </c>
+      <c r="L10">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="K11">
+        <v>6.93</v>
+      </c>
+      <c r="L11">
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10">
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12">
         <v>22.23</v>
       </c>
-      <c r="K10">
+      <c r="K12">
         <v>7.74</v>
       </c>
-      <c r="L10">
+      <c r="L12">
         <v>18.02</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="7" t="s">
+      <c r="N14" s="7" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="2">
-        <v>20000</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="2">
-        <v>30.88</v>
-      </c>
-      <c r="K13" s="2">
-        <v>11.04</v>
-      </c>
-      <c r="L13" s="2">
-        <v>23.21</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20000</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="1">
-        <v>50000</v>
-      </c>
-      <c r="J14" s="9">
-        <v>32.340000000000003</v>
-      </c>
-      <c r="K14" s="9">
-        <v>12.64</v>
-      </c>
-      <c r="L14" s="9">
-        <v>24.17</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="1">
-        <v>50000</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="1">
-        <v>70000</v>
-      </c>
-      <c r="J15" s="9">
-        <v>32.15</v>
-      </c>
-      <c r="K15" s="9">
-        <v>12.66</v>
-      </c>
-      <c r="L15" s="9">
-        <v>24.23</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="2">
+        <v>30.88</v>
+      </c>
+      <c r="K15" s="2">
+        <v>11.04</v>
+      </c>
+      <c r="L15" s="2">
+        <v>23.21</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
@@ -3523,275 +3469,391 @@
       <c r="E16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1">
+        <v>50000</v>
+      </c>
+      <c r="J16" s="9">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="K16" s="9">
+        <v>12.64</v>
+      </c>
+      <c r="L16" s="9">
+        <v>24.17</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="1">
+        <v>70000</v>
+      </c>
+      <c r="J17" s="9">
+        <v>32.15</v>
+      </c>
+      <c r="K17" s="9">
+        <v>12.66</v>
+      </c>
+      <c r="L17" s="9">
+        <v>24.23</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G18" s="1">
         <v>50000</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="H18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="1">
         <v>70000</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J18" s="5">
         <v>32.56</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K18" s="5">
         <v>12.97</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L18" s="5">
         <v>24.52</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="5">
+        <v>25.1</v>
+      </c>
+      <c r="K19" s="5">
+        <v>7.54</v>
+      </c>
+      <c r="L19" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20" s="5">
+        <v>31.9</v>
+      </c>
+      <c r="K20" s="5">
+        <v>12.64</v>
+      </c>
+      <c r="L20" s="5">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17">
+      <c r="H21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21">
         <v>33.6</v>
       </c>
-      <c r="K17">
+      <c r="K21">
         <v>15.81</v>
       </c>
-      <c r="L17">
+      <c r="L21">
         <v>24.94</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18">
+      <c r="H22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22">
         <v>30.13</v>
       </c>
-      <c r="K18">
+      <c r="K22">
         <v>11.84</v>
       </c>
-      <c r="L18">
+      <c r="L22">
         <v>22.29</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19">
-        <v>26.9</v>
-      </c>
-      <c r="K19">
-        <v>8.84</v>
-      </c>
-      <c r="L19">
-        <v>20.55</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20">
-        <v>25.3</v>
-      </c>
-      <c r="K20">
-        <v>8.27</v>
-      </c>
-      <c r="L20">
-        <v>19.309999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21">
-        <v>24.68</v>
-      </c>
-      <c r="K21">
-        <v>7.64</v>
-      </c>
-      <c r="L21">
-        <v>18.93</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22">
-        <v>25.56</v>
-      </c>
-      <c r="K22">
-        <v>8.35</v>
-      </c>
-      <c r="L22">
-        <v>19.54</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E23" s="1"/>
       <c r="H23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J23">
-        <v>27.9</v>
+        <v>26.9</v>
       </c>
       <c r="K23">
-        <v>9.06</v>
+        <v>8.84</v>
       </c>
       <c r="L23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1"/>
       <c r="H24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J24">
-        <v>26.82</v>
+        <v>25.3</v>
       </c>
       <c r="K24">
-        <v>8.89</v>
+        <v>8.27</v>
       </c>
       <c r="L24">
-        <v>20.43</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+        <v>19.309999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1"/>
       <c r="H25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J25">
-        <v>27.39</v>
+        <v>24.68</v>
       </c>
       <c r="K25">
-        <v>9.2100000000000009</v>
+        <v>7.64</v>
       </c>
       <c r="L25">
-        <v>20.8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+        <v>18.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1"/>
       <c r="H26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J26">
-        <v>25.23</v>
+        <v>25.56</v>
       </c>
       <c r="K26">
-        <v>8.98</v>
+        <v>8.35</v>
       </c>
       <c r="L26">
-        <v>18.04</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+        <v>19.54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E27" s="1"/>
       <c r="H27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J27">
+        <v>27.9</v>
+      </c>
+      <c r="K27">
+        <v>9.06</v>
+      </c>
+      <c r="L27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>26.82</v>
+      </c>
+      <c r="K28">
+        <v>8.89</v>
+      </c>
+      <c r="L28">
+        <v>20.43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29">
+        <v>27.39</v>
+      </c>
+      <c r="K29">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="L29">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30">
+        <v>25.23</v>
+      </c>
+      <c r="K30">
+        <v>8.98</v>
+      </c>
+      <c r="L30">
+        <v>18.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31">
         <v>20.399999999999999</v>
       </c>
-      <c r="K27">
+      <c r="K31">
         <v>6.91</v>
       </c>
-      <c r="L27">
+      <c r="L31">
         <v>15.91</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="H28" s="1"/>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="H32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>